<commit_message>
recording errors in SimpleMl
</commit_message>
<xml_diff>
--- a/RawData/OptimizationofHydrothermalACS.xlsx
+++ b/RawData/OptimizationofHydrothermalACS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward\OneDrive\Documents\University\Fourth Year\Thesis\HemicelluloseThesis\ExcelDataCollection\Complete\ThesisOnlyDataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="177" documentId="8_{BC9058C2-E3DB-452F-8DBF-66EF6A3D8E54}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B261DE03-913C-434D-B981-B9BF8B874291}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="8_{BC9058C2-E3DB-452F-8DBF-66EF6A3D8E54}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{9D88B15D-930B-4192-99CE-F8424392E369}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" activeTab="1" xr2:uid="{F7D4016F-954D-4B80-AFA5-87A3D2A0C639}"/>
   </bookViews>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9B104C-EE7C-484C-AB3E-2209443B4C18}">
   <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView topLeftCell="B33" workbookViewId="0">
-      <selection activeCell="S36" sqref="S36:S59"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3057,10 +3057,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47EE8DDF-C41D-4397-8FFD-DE7728229C53}">
-  <dimension ref="A1:Y26"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+      <selection activeCell="B12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3624,7 +3624,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B12" s="1">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C12">
         <v>15</v>
@@ -3663,18 +3663,18 @@
         <v>4.3295450000000004</v>
       </c>
       <c r="S12">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="T12">
-        <v>5221</v>
+        <v>2.72</v>
       </c>
       <c r="Y12">
-        <v>1.23</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B13" s="1">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="C13">
         <v>15</v>
@@ -3713,18 +3713,21 @@
         <v>4.3295450000000004</v>
       </c>
       <c r="S13">
-        <v>1.3</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="T13">
-        <v>2.72</v>
+        <v>0.36</v>
       </c>
       <c r="Y13">
-        <v>1.27</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>0</v>
+      </c>
       <c r="B14" s="1">
-        <v>220</v>
+        <v>170</v>
       </c>
       <c r="C14">
         <v>15</v>
@@ -3748,34 +3751,31 @@
         <v>7</v>
       </c>
       <c r="K14">
-        <v>1.659</v>
+        <v>0.36666670000000001</v>
       </c>
       <c r="L14">
-        <v>1.0777779999999999</v>
+        <v>1.81111</v>
       </c>
       <c r="M14">
-        <v>45</v>
+        <v>37.55555555555555</v>
       </c>
       <c r="N14">
-        <v>16.034089999999999</v>
+        <v>15</v>
       </c>
       <c r="O14">
-        <v>4.3295450000000004</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <v>1.0900000000000001</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <v>0.36</v>
+        <v>2.59</v>
       </c>
       <c r="Y14">
-        <v>0.23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A15">
-        <v>0</v>
-      </c>
       <c r="B15" s="1">
         <v>170</v>
       </c>
@@ -3816,13 +3816,13 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="T15">
-        <v>2.59</v>
+        <v>1</v>
       </c>
       <c r="Y15">
-        <v>0</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.4">
@@ -3845,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="J16">
         <v>7</v>
@@ -3866,13 +3866,13 @@
         <v>0</v>
       </c>
       <c r="S16">
-        <v>1.1200000000000001</v>
+        <v>1.51</v>
       </c>
       <c r="T16">
-        <v>1</v>
+        <v>4.21</v>
       </c>
       <c r="Y16">
-        <v>0.56000000000000005</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.4">
@@ -3895,7 +3895,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="J17">
         <v>7</v>
@@ -3916,13 +3916,13 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <v>1.51</v>
+        <v>1.56</v>
       </c>
       <c r="T17">
-        <v>4.21</v>
+        <v>5.45</v>
       </c>
       <c r="Y17">
-        <v>1.29</v>
+        <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.4">
@@ -3945,7 +3945,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="J18">
         <v>7</v>
@@ -3966,13 +3966,13 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>1.56</v>
+        <v>1.61</v>
       </c>
       <c r="T18">
-        <v>5.45</v>
+        <v>6.13</v>
       </c>
       <c r="Y18">
-        <v>2.0499999999999998</v>
+        <v>2.74</v>
       </c>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.4">
@@ -3995,7 +3995,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="1">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="J19">
         <v>7</v>
@@ -4016,13 +4016,13 @@
         <v>0</v>
       </c>
       <c r="S19">
-        <v>1.61</v>
+        <v>1.79</v>
       </c>
       <c r="T19">
-        <v>6.13</v>
+        <v>5.77</v>
       </c>
       <c r="Y19">
-        <v>2.74</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.4">
@@ -4045,7 +4045,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="1">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="J20">
         <v>7</v>
@@ -4066,18 +4066,18 @@
         <v>0</v>
       </c>
       <c r="S20">
-        <v>1.79</v>
+        <v>2.72</v>
       </c>
       <c r="T20">
-        <v>5.77</v>
+        <v>4.75</v>
       </c>
       <c r="Y20">
-        <v>2.99</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.4">
       <c r="B21" s="1">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="C21">
         <v>15</v>
@@ -4095,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="1">
-        <v>180</v>
+        <v>15</v>
       </c>
       <c r="J21">
         <v>7</v>
@@ -4116,18 +4116,18 @@
         <v>0</v>
       </c>
       <c r="S21">
-        <v>2.72</v>
+        <v>1.37</v>
       </c>
       <c r="T21">
-        <v>4.75</v>
+        <v>5.19</v>
       </c>
       <c r="Y21">
-        <v>2.67</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.4">
       <c r="B22" s="1">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="C22">
         <v>15</v>
@@ -4166,18 +4166,18 @@
         <v>0</v>
       </c>
       <c r="S22">
-        <v>1.37</v>
+        <v>1.48</v>
       </c>
       <c r="T22">
-        <v>5.19</v>
+        <v>6.08</v>
       </c>
       <c r="Y22">
-        <v>1.29</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.4">
       <c r="B23" s="1">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="C23">
         <v>15</v>
@@ -4216,18 +4216,18 @@
         <v>0</v>
       </c>
       <c r="S23">
-        <v>1.48</v>
+        <v>1.64</v>
       </c>
       <c r="T23">
-        <v>6.08</v>
+        <v>5.74</v>
       </c>
       <c r="Y23">
-        <v>2.09</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.4">
       <c r="B24" s="1">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C24">
         <v>15</v>
@@ -4266,18 +4266,18 @@
         <v>0</v>
       </c>
       <c r="S24">
-        <v>1.64</v>
+        <v>2.59</v>
       </c>
       <c r="T24">
-        <v>5.74</v>
+        <v>3.22</v>
       </c>
       <c r="Y24">
-        <v>2.83</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.4">
       <c r="B25" s="1">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="C25">
         <v>15</v>
@@ -4316,62 +4316,12 @@
         <v>0</v>
       </c>
       <c r="S25">
-        <v>2.59</v>
+        <v>1.96</v>
       </c>
       <c r="T25">
-        <v>3.22</v>
+        <v>0.92</v>
       </c>
       <c r="Y25">
-        <v>2.0299999999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.4">
-      <c r="B26" s="1">
-        <v>220</v>
-      </c>
-      <c r="C26">
-        <v>15</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0.59</v>
-      </c>
-      <c r="F26">
-        <v>37.5</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1">
-        <v>15</v>
-      </c>
-      <c r="J26">
-        <v>7</v>
-      </c>
-      <c r="K26">
-        <v>0.36666670000000001</v>
-      </c>
-      <c r="L26">
-        <v>1.81111</v>
-      </c>
-      <c r="M26">
-        <v>37.55555555555555</v>
-      </c>
-      <c r="N26">
-        <v>15</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="S26">
-        <v>1.96</v>
-      </c>
-      <c r="T26">
-        <v>0.92</v>
-      </c>
-      <c r="Y26">
         <v>0.67</v>
       </c>
     </row>

</xml_diff>